<commit_message>
saveAlbumForCurrentUser automation is on hold (code, test cases and test data is completed)
</commit_message>
<xml_diff>
--- a/TestData/SpotifyTestData.xlsx
+++ b/TestData/SpotifyTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abgoyal\Downloads\SpotifyAPIAutomation\1-automate-albums-endpoints\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E43535A-B1B6-4A85-AC2D-6C89AB9679DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA36E2C4-91A0-4E04-B165-BCDED87F7FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Albums" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Albums!$A$1:$J$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Albums!$A$1:$J$41</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="87">
   <si>
     <t>clientId</t>
   </si>
@@ -290,39 +290,6 @@
   </si>
   <si>
     <t>Invalid limit</t>
-  </si>
-  <si>
-    <t>TC_002_Albums_35</t>
-  </si>
-  <si>
-    <t>TC_002_Albums_36</t>
-  </si>
-  <si>
-    <t>TC_002_Albums_37</t>
-  </si>
-  <si>
-    <t>TC_002_Albums_38</t>
-  </si>
-  <si>
-    <t>TC_002_Albums_39</t>
-  </si>
-  <si>
-    <t>TC_002_Albums_40</t>
-  </si>
-  <si>
-    <t>TC_002_Albums_41</t>
-  </si>
-  <si>
-    <t>TC_002_Albums_42</t>
-  </si>
-  <si>
-    <t>TC_002_Albums_43</t>
-  </si>
-  <si>
-    <t>TC_002_Albums_44</t>
-  </si>
-  <si>
-    <t>test_saveAlbumForCurrentUser</t>
   </si>
 </sst>
 </file>
@@ -800,24 +767,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{859D71F6-8BF6-4ADF-A3D5-EDBBFEE55BBD}">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J45" sqref="J45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="20.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="23.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="8.77734375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
@@ -826,942 +793,769 @@
         <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2">
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2">
         <v>200</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>200</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G4" s="2">
-        <v>400</v>
-      </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="2">
+        <v>400</v>
+      </c>
+      <c r="I4" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="G5" s="2">
-        <v>400</v>
-      </c>
-      <c r="H5" s="2" t="s">
+      <c r="D5" s="7"/>
+      <c r="H5" s="2">
+        <v>400</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="B6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>401</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2">
-        <v>400</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="2">
+        <v>400</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="2">
         <v>401</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H9" s="2">
         <v>401</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="2">
-        <v>400</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="H10" s="2">
+        <v>400</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="2">
         <v>200</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="2">
-        <v>400</v>
-      </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="2">
+        <v>400</v>
+      </c>
+      <c r="I12" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="66">
       <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>200</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="79.2">
       <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="2">
-        <v>400</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="2">
+        <v>400</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>60</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="B15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>200</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="2">
-        <v>400</v>
-      </c>
-      <c r="H16" s="2" t="s">
+      <c r="H16" s="2">
+        <v>400</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>200</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="B18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>200</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>401</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="2">
-        <v>400</v>
-      </c>
-      <c r="H20" s="2" t="s">
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="2">
+        <v>400</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="2">
+      <c r="B21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="2">
         <v>401</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="I21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="2">
+      <c r="B22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H22" s="2">
         <v>401</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="2">
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="2">
         <v>200</v>
-      </c>
-      <c r="J23" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="B24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>200</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="J24" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="J24" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="2">
-        <v>400</v>
-      </c>
-      <c r="H25" s="2" t="s">
+      <c r="H25" s="2">
+        <v>400</v>
+      </c>
+      <c r="I25" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="J25" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="B26" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>401</v>
       </c>
-      <c r="H26" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="J26" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27" s="2" t="s">
+      <c r="B27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G27" s="2">
+      <c r="H27" s="2">
         <v>200</v>
-      </c>
-      <c r="J27" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="2">
+      <c r="B28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="2">
         <v>10</v>
       </c>
-      <c r="G28" s="2">
+      <c r="H28" s="2">
         <v>200</v>
-      </c>
-      <c r="J28" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F29" s="2">
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G29" s="2">
         <v>11.1</v>
       </c>
-      <c r="G29" s="2">
-        <v>400</v>
-      </c>
-      <c r="H29" s="2" t="s">
+      <c r="H29" s="2">
+        <v>400</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="J29" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="2" t="s">
+      <c r="B30" t="s">
+        <v>84</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G30" s="2">
-        <v>400</v>
-      </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="2">
+        <v>400</v>
+      </c>
+      <c r="I30" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="J30" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="2" t="s">
+      <c r="B31" t="s">
+        <v>84</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G31" s="2">
+      <c r="H31" s="2">
         <v>200</v>
-      </c>
-      <c r="J31" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="2">
+      <c r="B32" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="2">
         <v>10</v>
       </c>
-      <c r="G32" s="2">
+      <c r="H32" s="2">
         <v>200</v>
-      </c>
-      <c r="J32" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E33" s="2">
+      <c r="B33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="2">
         <v>11.1</v>
       </c>
-      <c r="G33" s="2">
-        <v>400</v>
-      </c>
-      <c r="H33" s="2" t="s">
+      <c r="H33" s="2">
+        <v>400</v>
+      </c>
+      <c r="I33" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="J33" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="B34" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G34" s="2">
-        <v>400</v>
-      </c>
-      <c r="H34" s="2" t="s">
+      <c r="H34" s="2">
+        <v>400</v>
+      </c>
+      <c r="I34" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="J34" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="2">
+      <c r="B35" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="2">
         <v>-1</v>
       </c>
-      <c r="G35" s="2">
-        <v>400</v>
-      </c>
-      <c r="H35" s="2" t="s">
+      <c r="H35" s="2">
+        <v>400</v>
+      </c>
+      <c r="I35" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="J35" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E36" s="2">
+      <c r="B36" t="s">
+        <v>84</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="2">
         <v>0</v>
       </c>
-      <c r="G36" s="2">
-        <v>400</v>
-      </c>
-      <c r="H36" s="2" t="s">
+      <c r="H36" s="2">
+        <v>400</v>
+      </c>
+      <c r="I36" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="J36" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E37" s="2">
+      <c r="B37" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="2">
         <v>51</v>
       </c>
-      <c r="G37" s="2">
-        <v>400</v>
-      </c>
-      <c r="H37" s="2" t="s">
+      <c r="H37" s="2">
+        <v>400</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="J37" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="2">
+      <c r="B38" t="s">
+        <v>84</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" s="2">
         <v>100</v>
       </c>
-      <c r="G38" s="2">
-        <v>400</v>
-      </c>
-      <c r="H38" s="2" t="s">
+      <c r="H38" s="2">
+        <v>400</v>
+      </c>
+      <c r="I38" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="J38" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="9"/>
-      <c r="G39" s="2">
-        <v>400</v>
-      </c>
-      <c r="H39" s="2" t="s">
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="H39" s="2">
+        <v>400</v>
+      </c>
+      <c r="I39" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="I39" s="2" t="s">
+      <c r="J39" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="J39" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="9"/>
-      <c r="G40" s="2">
+      <c r="B40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="9"/>
+      <c r="H40" s="2">
         <v>401</v>
       </c>
-      <c r="H40" s="2" t="s">
+      <c r="I40" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="J40" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="J40" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="9"/>
-      <c r="G41" s="2">
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="H41" s="2">
         <v>401</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I41" s="2" t="s">
+      <c r="J41" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="J41" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10">
-      <c r="A42" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="G42" s="2">
-        <v>400</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J42" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G43" s="2">
-        <v>200</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J43" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G44" s="2">
-        <v>400</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J44" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="66">
-      <c r="A45" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G45" s="2">
-        <v>200</v>
-      </c>
-      <c r="J45" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="79.2">
-      <c r="A46" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G46" s="2">
-        <v>400</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J46" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10">
-      <c r="A47" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G47" s="2">
-        <v>200</v>
-      </c>
-      <c r="J47" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10">
-      <c r="A48" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G48" s="2">
-        <v>400</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J48" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10">
-      <c r="A49" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G49" s="2">
-        <v>400</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J49" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G50" s="2">
-        <v>401</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J50" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10">
-      <c r="A51" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G51" s="2">
-        <v>401</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I51" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="J51" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>